<commit_message>
Remove White Spaces on News, Announcements, Course, Department. Separate Pending Alumni to Approved Alumni
</commit_message>
<xml_diff>
--- a/coordinator/excelFiles/alumni_data_report.xlsx
+++ b/coordinator/excelFiles/alumni_data_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>Student Number</t>
   </si>
@@ -86,31 +86,10 @@
     <t>Reyes</t>
   </si>
   <si>
-    <t>Andrei</t>
-  </si>
-  <si>
-    <t>Mercado</t>
-  </si>
-  <si>
     <t>Biya</t>
   </si>
   <si>
     <t>Sungit</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Benz</t>
-  </si>
-  <si>
-    <t>BSCS</t>
-  </si>
-  <si>
-    <t>Rudolf</t>
-  </si>
-  <si>
-    <t>Reindeer</t>
   </si>
 </sst>
 </file>
@@ -450,7 +429,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,7 +600,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>202013211</v>
+        <v>202119099</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
@@ -630,7 +609,7 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -639,76 +618,7 @@
         <v>11</v>
       </c>
       <c r="G8">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>202119099</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9">
         <v>2024</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <v>202011115</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
-        <v>201231231</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11">
-        <v>2022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>